<commit_message>
Mejorados casos de prueba en Excel
</commit_message>
<xml_diff>
--- a/Casos de prueba tarjeta de credito.xlsx
+++ b/Casos de prueba tarjeta de credito.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27932"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\b12s304\Documents\lpcl\cheat-sheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DA4CA2A1-DB01-49C7-AE21-770C59EB1AF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DD6BEBF-CEBD-4549-8C1D-A0291E5EB439}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,8 +27,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,19 +36,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="34">
   <si>
-    <t>P</t>
-  </si>
-  <si>
-    <t>i</t>
-  </si>
-  <si>
-    <t>n</t>
-  </si>
-  <si>
     <t>Salida</t>
-  </si>
-  <si>
-    <t>excel</t>
   </si>
   <si>
     <t>Total Abonos</t>
@@ -139,6 +125,18 @@
   <si>
     <t>ERROR: El valor de la compra debe ser mayor que cero</t>
   </si>
+  <si>
+    <t>Valor de la Compra</t>
+  </si>
+  <si>
+    <t>Tasa de Interés Mensual</t>
+  </si>
+  <si>
+    <t>Plazo en meses</t>
+  </si>
+  <si>
+    <t>Cuota Mensual</t>
+  </si>
 </sst>
 </file>
 
@@ -205,7 +203,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -218,6 +216,10 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Millares" xfId="1" builtinId="3"/>
@@ -536,13 +538,13 @@
   <dimension ref="A3:K136"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7109375" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="17.28515625" customWidth="1"/>
-    <col min="2" max="2" width="12.42578125" customWidth="1"/>
+    <col min="2" max="2" width="16.140625" customWidth="1"/>
     <col min="3" max="3" width="12" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12.5703125" customWidth="1"/>
     <col min="5" max="5" width="14.28515625" hidden="1" customWidth="1"/>
@@ -556,47 +558,47 @@
   <sheetData>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="B3" s="6" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="C3" s="6"/>
       <c r="D3" s="6"/>
       <c r="F3" s="7" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G3" s="7"/>
       <c r="H3" s="7"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B4" t="s">
-        <v>0</v>
-      </c>
-      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="8" t="s">
+        <v>30</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>31</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="F4" s="8" t="s">
+        <v>33</v>
+      </c>
+      <c r="G4" s="8" t="s">
         <v>1</v>
       </c>
-      <c r="D4" t="s">
+      <c r="H4" s="8" t="s">
         <v>2</v>
-      </c>
-      <c r="E4" t="s">
-        <v>3</v>
-      </c>
-      <c r="F4" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" t="s">
-        <v>6</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="B5" s="3">
         <v>200000</v>
       </c>
       <c r="C5" s="2">
@@ -640,9 +642,9 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B6">
+        <v>4</v>
+      </c>
+      <c r="B6" s="3">
         <v>850000</v>
       </c>
       <c r="C6" s="2">
@@ -656,7 +658,7 @@
         <v>52377.498639836558</v>
       </c>
       <c r="F6" s="1">
-        <f t="shared" ref="F6:F17" si="2">PMT(C6,D6,B6)*-1</f>
+        <f t="shared" ref="F6:F10" si="2">PMT(C6,D6,B6)*-1</f>
         <v>52377.498639836529</v>
       </c>
       <c r="G6" s="1">
@@ -685,6 +687,7 @@
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B7" s="3"/>
       <c r="C7" s="2"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
@@ -692,8 +695,9 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="5" t="s">
-        <v>24</v>
-      </c>
+        <v>20</v>
+      </c>
+      <c r="B8" s="3"/>
       <c r="C8" s="2"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
@@ -701,9 +705,9 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
-      </c>
-      <c r="B9">
+        <v>7</v>
+      </c>
+      <c r="B9" s="3">
         <v>90000</v>
       </c>
       <c r="C9" s="2">
@@ -715,7 +719,7 @@
       <c r="E9">
         <v>90000</v>
       </c>
-      <c r="F9">
+      <c r="F9" s="9">
         <v>90000</v>
       </c>
       <c r="G9" s="1">
@@ -745,9 +749,9 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10">
+        <v>5</v>
+      </c>
+      <c r="B10" s="3">
         <v>480000</v>
       </c>
       <c r="C10">
@@ -769,7 +773,7 @@
         <v>480000</v>
       </c>
       <c r="H10" s="1">
-        <f t="shared" ref="H10:H17" si="5">ROUND(G10-B10,2)</f>
+        <f t="shared" ref="H10" si="5">ROUND(G10-B10,2)</f>
         <v>0</v>
       </c>
       <c r="I10" t="str">
@@ -784,23 +788,25 @@
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
       <c r="F11" s="1"/>
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>25</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="B12" s="3"/>
       <c r="F12" s="1"/>
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B13">
+        <v>6</v>
+      </c>
+      <c r="B13" s="3">
         <v>50000</v>
       </c>
       <c r="C13" s="2">
@@ -814,7 +820,7 @@
         <v>6205.5821802692026</v>
       </c>
       <c r="F13" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
@@ -829,11 +835,14 @@
 Total Intereses: </v>
       </c>
     </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B14" s="3"/>
+    </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15">
+        <v>8</v>
+      </c>
+      <c r="B15" s="3">
         <v>0</v>
       </c>
       <c r="C15" s="2">
@@ -843,10 +852,10 @@
         <v>60</v>
       </c>
       <c r="E15" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="F15" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
@@ -863,9 +872,9 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16">
+        <v>9</v>
+      </c>
+      <c r="B16" s="3">
         <v>80000</v>
       </c>
       <c r="C16" s="2">
@@ -875,10 +884,10 @@
         <v>0</v>
       </c>
       <c r="E16" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="F16" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
@@ -895,9 +904,9 @@
     </row>
     <row r="17" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>14</v>
-      </c>
-      <c r="B17">
+        <v>10</v>
+      </c>
+      <c r="B17" s="3">
         <v>50000</v>
       </c>
       <c r="C17" s="2">
@@ -907,10 +916,10 @@
         <v>-10</v>
       </c>
       <c r="E17" t="s">
+        <v>24</v>
+      </c>
+      <c r="F17" s="1" t="s">
         <v>28</v>
-      </c>
-      <c r="F17" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
@@ -927,13 +936,13 @@
     </row>
     <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="G20" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="H20">
         <v>53000</v>
       </c>
       <c r="I20" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="J20">
         <v>10</v>
@@ -941,13 +950,13 @@
     </row>
     <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B21">
         <v>1</v>
       </c>
       <c r="G21" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="H21">
         <v>1</v>
@@ -955,33 +964,33 @@
     </row>
     <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="E22" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="H22" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="I22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="J22" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="K22" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
     </row>
     <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B23" s="3">
         <f>INDEX($A$5:$E$17,$B$21,5)</f>
@@ -996,7 +1005,7 @@
         <v>200000</v>
       </c>
       <c r="G23" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="H23" s="3">
         <f>INDEX($A$5:$E$17,$B$21,5)</f>
@@ -5537,5 +5546,6 @@
     <mergeCell ref="F3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>